<commit_message>
new changes in ops (ordercreation & orderpage & order form)
12/30/2024 new changes in ops (ordercreation & orderpage & order form)
</commit_message>
<xml_diff>
--- a/public/template/ATA National Title_sample_template.xlsx
+++ b/public/template/ATA National Title_sample_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tester\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C65C85-BD93-4AC7-BE2C-27676B1F95DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90B019B-F2D2-4CBD-8A4C-538DD0EB8F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="288" yWindow="768" windowWidth="22752" windowHeight="6816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="with_all_correctdata" sheetId="1" r:id="rId1"/>
@@ -120,10 +120,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
-  </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +261,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -447,8 +459,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFE699"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -629,9 +641,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -990,59 +1002,60 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="8" width="16" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="16" customWidth="1"/>
     <col min="12" max="12" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1050,40 +1063,40 @@
       <c r="A2" s="2">
         <v>45436</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>1213286</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1091,40 +1104,40 @@
       <c r="A3" s="2">
         <v>45439</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3">
         <v>2193289</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="3" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "new changes in ops (ordercreation & orderpage & order form)"
This reverts commit 2b346985827c5f1cc0421abf0dd74455991406a2.
</commit_message>
<xml_diff>
--- a/public/template/ATA National Title_sample_template.xlsx
+++ b/public/template/ATA National Title_sample_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tester\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90B019B-F2D2-4CBD-8A4C-538DD0EB8F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C65C85-BD93-4AC7-BE2C-27676B1F95DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="768" windowWidth="22752" windowHeight="6816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="with_all_correctdata" sheetId="1" r:id="rId1"/>
@@ -120,7 +120,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+  </numFmts>
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,21 +264,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -459,8 +447,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFE699"/>
-        <bgColor rgb="FF000000"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -641,9 +629,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1002,60 +990,59 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="16" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="8" width="16" customWidth="1"/>
     <col min="12" max="12" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1063,40 +1050,40 @@
       <c r="A2" s="2">
         <v>45436</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="1">
         <v>1213286</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1104,40 +1091,40 @@
       <c r="A3" s="2">
         <v>45439</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="1">
         <v>2193289</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reapply "new changes in ops (ordercreation & orderpage & order form)"
This reverts commit b94fd3cad26d1121e06137a219289729078b1709.
</commit_message>
<xml_diff>
--- a/public/template/ATA National Title_sample_template.xlsx
+++ b/public/template/ATA National Title_sample_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tester\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C65C85-BD93-4AC7-BE2C-27676B1F95DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90B019B-F2D2-4CBD-8A4C-538DD0EB8F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="288" yWindow="768" windowWidth="22752" windowHeight="6816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="with_all_correctdata" sheetId="1" r:id="rId1"/>
@@ -120,10 +120,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
-  </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +261,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -447,8 +459,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFE699"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -629,9 +641,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -990,59 +1002,60 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="8" width="16" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="16" customWidth="1"/>
     <col min="12" max="12" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1050,40 +1063,40 @@
       <c r="A2" s="2">
         <v>45436</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>1213286</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1091,40 +1104,40 @@
       <c r="A3" s="2">
         <v>45439</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3">
         <v>2193289</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="3" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>